<commit_message>
Tracking bartonski parado, stephen funcionando
</commit_message>
<xml_diff>
--- a/AlejandroAlonso/results/excels/tracking_short_denoise.xlsx
+++ b/AlejandroAlonso/results/excels/tracking_short_denoise.xlsx
@@ -530,7 +530,47 @@
       </c>
       <c r="T1" t="inlineStr">
         <is>
+          <t>Bola num 47</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Bola num 49</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
           <t>Bola num 50</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>Bola num 82</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>Bola num 84</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>Bola num 135</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>Bola num 136</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>Bola num 137</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>Bola num 138</t>
         </is>
       </c>
     </row>
@@ -631,6 +671,86 @@
         </is>
       </c>
       <c r="U2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -1181,9 +1301,21 @@
         <v>1015</v>
       </c>
       <c r="T29" t="n">
+        <v>537</v>
+      </c>
+      <c r="U29" t="n">
+        <v>1199</v>
+      </c>
+      <c r="V29" t="n">
+        <v>567</v>
+      </c>
+      <c r="W29" t="n">
+        <v>942</v>
+      </c>
+      <c r="X29" t="n">
         <v>654</v>
       </c>
-      <c r="U29" t="n">
+      <c r="Y29" t="n">
         <v>867</v>
       </c>
     </row>
@@ -1222,9 +1354,21 @@
         <v>1011</v>
       </c>
       <c r="T30" t="n">
+        <v>546</v>
+      </c>
+      <c r="U30" t="n">
+        <v>1231</v>
+      </c>
+      <c r="V30" t="n">
+        <v>560</v>
+      </c>
+      <c r="W30" t="n">
+        <v>914</v>
+      </c>
+      <c r="X30" t="n">
         <v>664</v>
       </c>
-      <c r="U30" t="n">
+      <c r="Y30" t="n">
         <v>900</v>
       </c>
     </row>
@@ -1256,6 +1400,12 @@
       <c r="S31" t="n">
         <v>987</v>
       </c>
+      <c r="T31" t="n">
+        <v>545</v>
+      </c>
+      <c r="U31" t="n">
+        <v>1239</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1532,6 +1682,18 @@
       <c r="M43" t="n">
         <v>1203</v>
       </c>
+      <c r="Z43" t="n">
+        <v>639</v>
+      </c>
+      <c r="AA43" t="n">
+        <v>1196</v>
+      </c>
+      <c r="AB43" t="n">
+        <v>606</v>
+      </c>
+      <c r="AC43" t="n">
+        <v>841</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1549,6 +1711,18 @@
       <c r="M44" t="n">
         <v>1217</v>
       </c>
+      <c r="Z44" t="n">
+        <v>638</v>
+      </c>
+      <c r="AA44" t="n">
+        <v>1217</v>
+      </c>
+      <c r="AB44" t="n">
+        <v>596</v>
+      </c>
+      <c r="AC44" t="n">
+        <v>817</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1566,6 +1740,18 @@
       <c r="M45" t="n">
         <v>1148</v>
       </c>
+      <c r="Z45" t="n">
+        <v>645</v>
+      </c>
+      <c r="AA45" t="n">
+        <v>1223</v>
+      </c>
+      <c r="AB45" t="n">
+        <v>610</v>
+      </c>
+      <c r="AC45" t="n">
+        <v>786</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1583,6 +1769,18 @@
       <c r="M46" t="n">
         <v>1144</v>
       </c>
+      <c r="Z46" t="n">
+        <v>639</v>
+      </c>
+      <c r="AA46" t="n">
+        <v>1218</v>
+      </c>
+      <c r="AB46" t="n">
+        <v>609</v>
+      </c>
+      <c r="AC46" t="n">
+        <v>773</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1600,6 +1798,12 @@
       <c r="M47" t="n">
         <v>1194</v>
       </c>
+      <c r="AB47" t="n">
+        <v>607</v>
+      </c>
+      <c r="AC47" t="n">
+        <v>765</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1617,6 +1821,12 @@
       <c r="M48" t="n">
         <v>1180</v>
       </c>
+      <c r="AB48" t="n">
+        <v>611</v>
+      </c>
+      <c r="AC48" t="n">
+        <v>763</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1634,6 +1844,18 @@
       <c r="M49" t="n">
         <v>1162</v>
       </c>
+      <c r="Z49" t="n">
+        <v>605</v>
+      </c>
+      <c r="AA49" t="n">
+        <v>1176</v>
+      </c>
+      <c r="AB49" t="n">
+        <v>614</v>
+      </c>
+      <c r="AC49" t="n">
+        <v>764</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1651,6 +1873,12 @@
       <c r="M50" t="n">
         <v>1137</v>
       </c>
+      <c r="AB50" t="n">
+        <v>617</v>
+      </c>
+      <c r="AC50" t="n">
+        <v>772</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1668,6 +1896,18 @@
       <c r="M51" t="n">
         <v>1105</v>
       </c>
+      <c r="Z51" t="n">
+        <v>456</v>
+      </c>
+      <c r="AA51" t="n">
+        <v>1095</v>
+      </c>
+      <c r="AB51" t="n">
+        <v>622</v>
+      </c>
+      <c r="AC51" t="n">
+        <v>785</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1685,6 +1925,18 @@
       <c r="M52" t="n">
         <v>1057</v>
       </c>
+      <c r="Z52" t="n">
+        <v>597</v>
+      </c>
+      <c r="AA52" t="n">
+        <v>1063</v>
+      </c>
+      <c r="AB52" t="n">
+        <v>627</v>
+      </c>
+      <c r="AC52" t="n">
+        <v>804</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1702,6 +1954,12 @@
       <c r="M53" t="n">
         <v>1025</v>
       </c>
+      <c r="Z53" t="n">
+        <v>630</v>
+      </c>
+      <c r="AA53" t="n">
+        <v>829</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1719,6 +1977,12 @@
       <c r="M54" t="n">
         <v>995</v>
       </c>
+      <c r="Z54" t="n">
+        <v>634</v>
+      </c>
+      <c r="AA54" t="n">
+        <v>858</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1730,6 +1994,12 @@
       <c r="M55" t="n">
         <v>996</v>
       </c>
+      <c r="Z55" t="n">
+        <v>532</v>
+      </c>
+      <c r="AA55" t="n">
+        <v>881</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1752,6 +2022,12 @@
       <c r="C57" t="n">
         <v>867</v>
       </c>
+      <c r="Z57" t="n">
+        <v>500</v>
+      </c>
+      <c r="AA57" t="n">
+        <v>1213</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1763,6 +2039,12 @@
       <c r="C58" t="n">
         <v>1243</v>
       </c>
+      <c r="Z58" t="n">
+        <v>507</v>
+      </c>
+      <c r="AA58" t="n">
+        <v>1196</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1774,6 +2056,12 @@
       <c r="C59" t="n">
         <v>1238</v>
       </c>
+      <c r="Z59" t="n">
+        <v>516</v>
+      </c>
+      <c r="AA59" t="n">
+        <v>1182</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1857,6 +2145,30 @@
       <c r="C66" t="n">
         <v>852</v>
       </c>
+      <c r="AD66" t="n">
+        <v>573</v>
+      </c>
+      <c r="AE66" t="n">
+        <v>1427</v>
+      </c>
+      <c r="AF66" t="n">
+        <v>581</v>
+      </c>
+      <c r="AG66" t="n">
+        <v>1362</v>
+      </c>
+      <c r="AH66" t="n">
+        <v>703</v>
+      </c>
+      <c r="AI66" t="n">
+        <v>1127</v>
+      </c>
+      <c r="AJ66" t="n">
+        <v>569</v>
+      </c>
+      <c r="AK66" t="n">
+        <v>1023</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -1873,6 +2185,18 @@
       </c>
       <c r="M67" t="n">
         <v>1048</v>
+      </c>
+      <c r="AH67" t="n">
+        <v>705</v>
+      </c>
+      <c r="AI67" t="n">
+        <v>1150</v>
+      </c>
+      <c r="AJ67" t="n">
+        <v>530</v>
+      </c>
+      <c r="AK67" t="n">
+        <v>776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>